<commit_message>
Added new files to the test automation framework
</commit_message>
<xml_diff>
--- a/Framework1/src/resource/java/testData/testData.xlsx
+++ b/Framework1/src/resource/java/testData/testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -35,16 +35,10 @@
     <t>cxvjcvxzjcvj</t>
   </si>
   <si>
-    <t>testdata55</t>
-  </si>
-  <si>
-    <t>testdata56</t>
-  </si>
-  <si>
-    <t>admin95</t>
-  </si>
-  <si>
-    <t>admin96</t>
+    <t>data45</t>
+  </si>
+  <si>
+    <t>bread88</t>
   </si>
 </sst>
 </file>
@@ -438,15 +432,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,15 +457,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>